<commit_message>
Bit more work done on the design
</commit_message>
<xml_diff>
--- a/Figures/TopDownDesign.xlsx
+++ b/Figures/TopDownDesign.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsmoffat/Documents/Comp4ProjectReport/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="27240" windowHeight="14900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
-    <t>Ordr</t>
-  </si>
-  <si>
     <t>MainMenu</t>
   </si>
   <si>
@@ -81,16 +78,41 @@
   </si>
   <si>
     <t>Show Contents with search</t>
+  </si>
+  <si>
+    <t>  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -113,8 +135,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -122,7 +146,9 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,7 +427,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection sqref="A1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -420,7 +446,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -441,84 +467,84 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
       <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="L3" t="s">
+      <c r="P3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" t="s">
-        <v>16</v>
-      </c>
-      <c r="P3" t="s">
-        <v>17</v>
-      </c>
       <c r="Q3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -530,6 +556,8 @@
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="O2:Q2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>